<commit_message>
git update powershell finished
</commit_message>
<xml_diff>
--- a/data/Upload/A.V.O.D. KURUTULMUŞ GIDA VE TARIM ÜRÜNLERİ SANAYİ TİCARET A.Ş.(10.05.2023).xlsx
+++ b/data/Upload/A.V.O.D. KURUTULMUŞ GIDA VE TARIM ÜRÜNLERİ SANAYİ TİCARET A.Ş.(10.05.2023).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SnorlaX\Downloads\at\Capstone\data\Upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5AEC5092-6929-4664-ABBF-D9EE392D6454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{853A27F4-505A-4E1E-93D1-A748502606EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="5025" windowWidth="28800" windowHeight="15435"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15435"/>
   </bookViews>
   <sheets>
     <sheet name="A.V.O.D. KURUTULMUŞ GIDA VE TAR" sheetId="2" r:id="rId1"/>

</xml_diff>